<commit_message>
New page: director detail
</commit_message>
<xml_diff>
--- a/MyProjectTracking.xlsx
+++ b/MyProjectTracking.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pduy8\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pduy8\OneDrive\Desktop\IntelliJ_IDEA_WorkSpace\PROJECT_SWP391_BookingCinemaTicket\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19395" windowHeight="11595"/>
+    <workbookView minimized="1" xWindow="-105" yWindow="-105" windowWidth="19395" windowHeight="11595"/>
   </bookViews>
   <sheets>
     <sheet name="RMS" sheetId="31" r:id="rId1"/>
     <sheet name="Params" sheetId="32" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RMS!$A$1:$I$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RMS!$A$1:$I$15</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -235,7 +235,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="72">
   <si>
     <t>In Charge</t>
   </si>
@@ -261,9 +261,6 @@
     <t>HaTH</t>
   </si>
   <si>
-    <t>AnhPT</t>
-  </si>
-  <si>
     <t>RDS</t>
   </si>
   <si>
@@ -274,9 +271,6 @@
   </si>
   <si>
     <t>Iteration 3</t>
-  </si>
-  <si>
-    <t>Blog Details</t>
   </si>
   <si>
     <t>Posts List</t>
@@ -831,12 +825,6 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -851,6 +839,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1213,11 +1207,11 @@
   <sheetPr>
     <outlinePr summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O3" sqref="O3"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1239,28 +1233,28 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I1" s="17" t="s">
         <v>1</v>
@@ -1268,22 +1262,22 @@
       <c r="J1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="K1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="38" t="s">
-        <v>61</v>
+      <c r="L1" s="36" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D2" s="29">
         <f>VLOOKUP(C2,Params!$K$2:$N$9,4,FALSE)</f>
@@ -1291,26 +1285,26 @@
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J2" s="6"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="35"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="33"/>
     </row>
     <row r="3" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D3" s="29">
         <f>VLOOKUP(C3,Params!$K$2:$N$9,4,FALSE)</f>
@@ -1318,26 +1312,26 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="8"/>
-      <c r="I3" s="39" t="s">
-        <v>28</v>
+      <c r="I3" s="37" t="s">
+        <v>26</v>
       </c>
       <c r="J3" s="6"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="37"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="35"/>
     </row>
     <row r="4" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D4" s="29">
         <f>VLOOKUP(C4,Params!$K$2:$N$9,4,FALSE)</f>
@@ -1345,26 +1339,26 @@
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="6"/>
-      <c r="I4" s="39" t="s">
-        <v>28</v>
+      <c r="I4" s="37" t="s">
+        <v>26</v>
       </c>
       <c r="J4" s="6"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="37"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="35"/>
     </row>
     <row r="5" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>67</v>
-      </c>
       <c r="C5" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D5" s="29">
         <f>VLOOKUP(C5,Params!$K$2:$N$9,4,FALSE)</f>
@@ -1372,26 +1366,26 @@
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="6"/>
-      <c r="I5" s="39" t="s">
-        <v>28</v>
+      <c r="I5" s="37" t="s">
+        <v>26</v>
       </c>
       <c r="J5" s="6"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="37"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="35"/>
     </row>
     <row r="6" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D6" s="29">
         <f>VLOOKUP(C6,Params!$K$2:$N$9,4,FALSE)</f>
@@ -1399,26 +1393,26 @@
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="9"/>
-      <c r="I6" s="39" t="s">
-        <v>28</v>
+      <c r="I6" s="37" t="s">
+        <v>26</v>
       </c>
       <c r="J6" s="6"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="37"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="35"/>
     </row>
     <row r="7" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D7" s="29">
         <f>VLOOKUP(C7,Params!$K$2:$N$9,4,FALSE)</f>
@@ -1426,119 +1420,121 @@
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="9"/>
-      <c r="I7" s="39" t="s">
-        <v>28</v>
+      <c r="I7" s="37" t="s">
+        <v>26</v>
       </c>
       <c r="J7" s="6"/>
-      <c r="K7" s="36"/>
-      <c r="L7" s="37"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="35"/>
     </row>
     <row r="8" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="29">
         <f>VLOOKUP(C8,Params!$K$2:$N$9,4,FALSE)</f>
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="9"/>
-      <c r="I8" s="39" t="s">
-        <v>28</v>
+      <c r="I8" s="37" t="s">
+        <v>26</v>
       </c>
       <c r="J8" s="6"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="37"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="35">
+        <v>540</v>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>13</v>
+      <c r="A9" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D9" s="29">
         <f>VLOOKUP(C9,Params!$K$2:$N$9,4,FALSE)</f>
         <v>60</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9" s="36"/>
-      <c r="L9" s="37"/>
+        <v>19</v>
+      </c>
+      <c r="K9" s="34"/>
+      <c r="L9" s="35"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D10" s="29">
         <f>VLOOKUP(C10,Params!$K$2:$N$9,4,FALSE)</f>
         <v>60</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="34"/>
+      <c r="L10" s="35"/>
+    </row>
+    <row r="11" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10" s="36"/>
-      <c r="L10" s="37"/>
-    </row>
-    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>15</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D11" s="29">
         <f>VLOOKUP(C11,Params!$K$2:$N$9,4,FALSE)</f>
@@ -1548,155 +1544,125 @@
         <v>11</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K11" s="36"/>
-      <c r="L11" s="37"/>
-    </row>
-    <row r="12" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="K11" s="34"/>
+      <c r="L11" s="35"/>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D12" s="29">
         <f>VLOOKUP(C12,Params!$K$2:$N$9,4,FALSE)</f>
         <v>60</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H12" s="9"/>
       <c r="I12" s="14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K12" s="36"/>
-      <c r="L12" s="37"/>
-    </row>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="K12" s="34"/>
+      <c r="L12" s="35"/>
+    </row>
+    <row r="13" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D13" s="29">
         <f>VLOOKUP(C13,Params!$K$2:$N$9,4,FALSE)</f>
         <v>60</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K13" s="36"/>
-      <c r="L13" s="37"/>
-    </row>
-    <row r="14" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="K13" s="34"/>
+      <c r="L13" s="35"/>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D14" s="29">
         <f>VLOOKUP(C14,Params!$K$2:$N$9,4,FALSE)</f>
         <v>60</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H14" s="9"/>
       <c r="I14" s="14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K14" s="36"/>
-      <c r="L14" s="37"/>
-    </row>
-    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="29">
-        <f>VLOOKUP(C15,Params!$K$2:$N$9,4,FALSE)</f>
-        <v>60</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K15" s="36"/>
-      <c r="L15" s="35"/>
+        <v>19</v>
+      </c>
+      <c r="K14" s="34"/>
+      <c r="L14" s="33"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
+      <c r="A16" s="11"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
@@ -1705,27 +1671,24 @@
       <c r="A18" s="11"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
+      <c r="A19" s="12"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
+      <c r="A20" s="13"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:I16"/>
+  <autoFilter ref="A1:I15"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H15 E2:E15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E14 G2:H14">
       <formula1>"Not Yet, Iteration 1, Iteration 2, Iteration 3"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J14">
       <formula1>"Not Yet, Iteration 2, Iteration 3"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I14">
       <formula1>"To Do, Doing, Done, Cancelled"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1739,7 +1702,7 @@
           <x14:formula1>
             <xm:f>Params!$K$3:$K$9</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C15</xm:sqref>
+          <xm:sqref>C2:C14</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1774,39 +1737,39 @@
   <sheetData>
     <row r="1" spans="2:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K2" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="N2" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="N2" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="O2" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="P2" s="31"/>
+      <c r="O2" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="38"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K3" s="22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L3" s="23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="M3" s="24">
         <v>2</v>
@@ -1814,21 +1777,21 @@
       <c r="N3" s="24">
         <v>60</v>
       </c>
-      <c r="O3" s="32" t="str">
+      <c r="O3" s="39" t="str">
         <f>L3 &amp; " fields OR " &amp; M3 &amp; " trans"</f>
         <v>3-5 fields OR 2 trans</v>
       </c>
-      <c r="P3" s="32"/>
+      <c r="P3" s="39"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="26" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K4" s="22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L4" s="23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M4" s="24">
         <v>3</v>
@@ -1836,21 +1799,21 @@
       <c r="N4" s="24">
         <v>90</v>
       </c>
-      <c r="O4" s="32" t="str">
+      <c r="O4" s="39" t="str">
         <f t="shared" ref="O4:O9" si="0">L4 &amp; " fields OR " &amp; M4 &amp; " trans"</f>
         <v>6-7 fields OR 3 trans</v>
       </c>
-      <c r="P4" s="32"/>
+      <c r="P4" s="39"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K5" s="22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L5" s="23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M5" s="24">
         <v>4</v>
@@ -1858,21 +1821,21 @@
       <c r="N5" s="24">
         <v>120</v>
       </c>
-      <c r="O5" s="32" t="str">
+      <c r="O5" s="39" t="str">
         <f t="shared" si="0"/>
         <v>8-9 fields OR 4 trans</v>
       </c>
-      <c r="P5" s="32"/>
+      <c r="P5" s="39"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K6" s="22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L6" s="23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M6" s="24">
         <v>5</v>
@@ -1889,10 +1852,10 @@
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="25"/>
       <c r="K7" s="22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L7" s="23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M7" s="24">
         <v>6</v>
@@ -1908,13 +1871,13 @@
     </row>
     <row r="8" spans="2:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B8" s="20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K8" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L8" s="23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M8" s="24">
         <v>7</v>
@@ -1930,16 +1893,16 @@
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K9" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L9" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="M9" s="24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="N9" s="24">
         <v>240</v>
@@ -1952,17 +1915,17 @@
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="K10" s="19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="K14" s="27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New feature: pagination for movie category, movice search, movie showing
</commit_message>
<xml_diff>
--- a/MyProjectTracking.xlsx
+++ b/MyProjectTracking.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="-105" yWindow="-105" windowWidth="19395" windowHeight="11595"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19395" windowHeight="11595"/>
   </bookViews>
   <sheets>
     <sheet name="RMS" sheetId="31" r:id="rId1"/>
@@ -1210,8 +1210,8 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1277,11 +1277,11 @@
         <v>60</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D2" s="29">
         <f>VLOOKUP(C2,Params!$K$2:$N$9,4,FALSE)</f>
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="4" t="s">
@@ -1439,11 +1439,11 @@
         <v>71</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D8" s="29">
         <f>VLOOKUP(C8,Params!$K$2:$N$9,4,FALSE)</f>
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
@@ -1457,7 +1457,7 @@
       <c r="J8" s="6"/>
       <c r="K8" s="34"/>
       <c r="L8" s="35">
-        <v>540</v>
+        <v>720</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1715,7 +1715,7 @@
   <dimension ref="B1:P22"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V15" sqref="V15"/>
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
New feature: encrypting passwords during login and registration
</commit_message>
<xml_diff>
--- a/MyProjectTracking.xlsx
+++ b/MyProjectTracking.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Params" sheetId="32" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RMS!$A$1:$I$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RMS!$A$1:$I$12</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -235,7 +235,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="68">
   <si>
     <t>In Charge</t>
   </si>
@@ -258,9 +258,6 @@
     <t>..</t>
   </si>
   <si>
-    <t>HaTH</t>
-  </si>
-  <si>
     <t>RDS</t>
   </si>
   <si>
@@ -273,27 +270,15 @@
     <t>Iteration 3</t>
   </si>
   <si>
-    <t>Posts List</t>
-  </si>
-  <si>
     <t>Post Details</t>
   </si>
   <si>
-    <t>Users List</t>
-  </si>
-  <si>
-    <t>User Details</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
     <t>TuanNV</t>
   </si>
   <si>
-    <t>ThuyTT</t>
-  </si>
-  <si>
     <t>Not Yet</t>
   </si>
   <si>
@@ -304,9 +289,6 @@
   </si>
   <si>
     <t>Setting List</t>
-  </si>
-  <si>
-    <t>Setting Details</t>
   </si>
   <si>
     <t>Done-In</t>
@@ -459,6 +441,12 @@
   <si>
     <t>As a user, I want to see which seats for that movie are mine and which are others so that I can easily choose.</t>
   </si>
+  <si>
+    <t>Movie category</t>
+  </si>
+  <si>
+    <t>As a user, I want to see movies filtered by showing or comming soon so that I can easily choose.</t>
+  </si>
 </sst>
 </file>
 
@@ -467,11 +455,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -734,117 +729,120 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="4" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="4" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="5" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="5" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1207,11 +1205,11 @@
   <sheetPr>
     <outlinePr summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1233,28 +1231,28 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I1" s="17" t="s">
         <v>1</v>
@@ -1266,18 +1264,18 @@
         <v>4</v>
       </c>
       <c r="L1" s="36" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D2" s="29">
         <f>VLOOKUP(C2,Params!$K$2:$N$9,4,FALSE)</f>
@@ -1285,12 +1283,12 @@
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="14" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J2" s="6"/>
       <c r="K2" s="32"/>
@@ -1301,10 +1299,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D3" s="29">
         <f>VLOOKUP(C3,Params!$K$2:$N$9,4,FALSE)</f>
@@ -1312,12 +1310,12 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="8"/>
       <c r="I3" s="37" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="32"/>
@@ -1325,26 +1323,26 @@
     </row>
     <row r="4" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D4" s="29">
         <f>VLOOKUP(C4,Params!$K$2:$N$9,4,FALSE)</f>
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="6"/>
       <c r="I4" s="37" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J4" s="6"/>
       <c r="K4" s="32"/>
@@ -1352,26 +1350,26 @@
     </row>
     <row r="5" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D5" s="29">
         <f>VLOOKUP(C5,Params!$K$2:$N$9,4,FALSE)</f>
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="6"/>
       <c r="I5" s="37" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J5" s="6"/>
       <c r="K5" s="32"/>
@@ -1379,13 +1377,13 @@
     </row>
     <row r="6" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D6" s="29">
         <f>VLOOKUP(C6,Params!$K$2:$N$9,4,FALSE)</f>
@@ -1393,12 +1391,12 @@
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="9"/>
       <c r="I6" s="37" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J6" s="6"/>
       <c r="K6" s="34"/>
@@ -1406,13 +1404,13 @@
     </row>
     <row r="7" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D7" s="29">
         <f>VLOOKUP(C7,Params!$K$2:$N$9,4,FALSE)</f>
@@ -1420,12 +1418,12 @@
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="9"/>
       <c r="I7" s="37" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J7" s="6"/>
       <c r="K7" s="34"/>
@@ -1433,13 +1431,13 @@
     </row>
     <row r="8" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D8" s="29">
         <f>VLOOKUP(C8,Params!$K$2:$N$9,4,FALSE)</f>
@@ -1447,248 +1445,143 @@
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="9"/>
       <c r="I8" s="37" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J8" s="6"/>
       <c r="K8" s="34"/>
       <c r="L8" s="35">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D9" s="29">
         <f>VLOOKUP(C9,Params!$K$2:$N$9,4,FALSE)</f>
-        <v>60</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="G9" s="3"/>
       <c r="H9" s="9"/>
-      <c r="I9" s="14" t="s">
+      <c r="I9" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="J9" s="6"/>
       <c r="K9" s="34"/>
       <c r="L9" s="35"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D10" s="29">
         <f>VLOOKUP(C10,Params!$K$2:$N$9,4,FALSE)</f>
         <v>60</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="14" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K10" s="34"/>
       <c r="L10" s="35"/>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D11" s="29">
         <f>VLOOKUP(C11,Params!$K$2:$N$9,4,FALSE)</f>
         <v>60</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="14" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K11" s="34"/>
       <c r="L11" s="35"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="29">
-        <f>VLOOKUP(C12,Params!$K$2:$N$9,4,FALSE)</f>
-        <v>60</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K12" s="34"/>
-      <c r="L12" s="35"/>
-    </row>
-    <row r="13" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="29">
-        <f>VLOOKUP(C13,Params!$K$2:$N$9,4,FALSE)</f>
-        <v>60</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K13" s="34"/>
-      <c r="L13" s="35"/>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="29">
-        <f>VLOOKUP(C14,Params!$K$2:$N$9,4,FALSE)</f>
-        <v>60</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" s="9"/>
-      <c r="I14" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K14" s="34"/>
-      <c r="L14" s="33"/>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
+      <c r="A15" s="11"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
+      <c r="A16" s="12"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
+      <c r="A17" s="13"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
+      <c r="A18" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I15"/>
+  <autoFilter ref="A1:I12"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E14 G2:H14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E11 G2:H11">
       <formula1>"Not Yet, Iteration 1, Iteration 2, Iteration 3"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J11">
       <formula1>"Not Yet, Iteration 2, Iteration 3"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I11">
       <formula1>"To Do, Doing, Done, Cancelled"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1702,7 +1595,7 @@
           <x14:formula1>
             <xm:f>Params!$K$3:$K$9</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C14</xm:sqref>
+          <xm:sqref>C2:C11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1714,7 +1607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P22"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
@@ -1737,39 +1630,39 @@
   <sheetData>
     <row r="1" spans="2:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="20" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="25" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="L2" s="21" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="M2" s="21" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="N2" s="21" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="O2" s="38" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="P2" s="38"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="26" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="K3" s="22" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="L3" s="23" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="M3" s="24">
         <v>2</v>
@@ -1785,13 +1678,13 @@
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="26" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="K4" s="22" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="L4" s="23" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="M4" s="24">
         <v>3</v>
@@ -1807,13 +1700,13 @@
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="25" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="K5" s="22" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="L5" s="23" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="M5" s="24">
         <v>4</v>
@@ -1829,13 +1722,13 @@
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="25" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="K6" s="22" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="L6" s="23" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="M6" s="24">
         <v>5</v>
@@ -1852,10 +1745,10 @@
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="25"/>
       <c r="K7" s="22" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="L7" s="23" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="M7" s="24">
         <v>6</v>
@@ -1871,13 +1764,13 @@
     </row>
     <row r="8" spans="2:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B8" s="20" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="K8" s="22" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="L8" s="23" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="M8" s="24">
         <v>7</v>
@@ -1893,16 +1786,16 @@
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="27" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="K9" s="22" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="L9" s="24" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="M9" s="24" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="N9" s="24">
         <v>240</v>
@@ -1915,17 +1808,17 @@
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="K10" s="19" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="K14" s="27" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="27" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix theme: change English to Viet Nam
</commit_message>
<xml_diff>
--- a/MyProjectTracking.xlsx
+++ b/MyProjectTracking.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19395" windowHeight="11595"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19395" windowHeight="11595" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RMS" sheetId="31" r:id="rId1"/>
@@ -235,7 +235,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="66">
   <si>
     <t>In Charge</t>
   </si>
@@ -252,9 +252,6 @@
     <t>Update Details</t>
   </si>
   <si>
-    <t>KienNT</t>
-  </si>
-  <si>
     <t>..</t>
   </si>
   <si>
@@ -264,13 +261,7 @@
     <t>Home Page</t>
   </si>
   <si>
-    <t>Iteration 2</t>
-  </si>
-  <si>
     <t>Iteration 3</t>
-  </si>
-  <si>
-    <t>Post Details</t>
   </si>
   <si>
     <t>Description</t>
@@ -447,6 +438,9 @@
   <si>
     <t>As a user, I want to see movies filtered by showing or comming soon so that I can easily choose.</t>
   </si>
+  <si>
+    <t>Register confirm</t>
+  </si>
 </sst>
 </file>
 
@@ -455,11 +449,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -729,116 +730,119 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="4" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="4" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="5" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="5" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1207,9 +1211,9 @@
   </sheetPr>
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N23" sqref="N23"/>
+      <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,28 +1235,28 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>19</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I1" s="17" t="s">
         <v>1</v>
@@ -1264,18 +1268,18 @@
         <v>4</v>
       </c>
       <c r="L1" s="36" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D2" s="29">
         <f>VLOOKUP(C2,Params!$K$2:$N$9,4,FALSE)</f>
@@ -1283,12 +1287,12 @@
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J2" s="6"/>
       <c r="K2" s="32"/>
@@ -1299,10 +1303,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D3" s="29">
         <f>VLOOKUP(C3,Params!$K$2:$N$9,4,FALSE)</f>
@@ -1310,12 +1314,12 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="8"/>
       <c r="I3" s="37" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="32"/>
@@ -1323,13 +1327,13 @@
     </row>
     <row r="4" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D4" s="29">
         <f>VLOOKUP(C4,Params!$K$2:$N$9,4,FALSE)</f>
@@ -1337,12 +1341,12 @@
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="6"/>
       <c r="I4" s="37" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J4" s="6"/>
       <c r="K4" s="32"/>
@@ -1350,13 +1354,13 @@
     </row>
     <row r="5" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D5" s="29">
         <f>VLOOKUP(C5,Params!$K$2:$N$9,4,FALSE)</f>
@@ -1364,12 +1368,12 @@
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="6"/>
       <c r="I5" s="37" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J5" s="6"/>
       <c r="K5" s="32"/>
@@ -1377,13 +1381,13 @@
     </row>
     <row r="6" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D6" s="29">
         <f>VLOOKUP(C6,Params!$K$2:$N$9,4,FALSE)</f>
@@ -1391,12 +1395,12 @@
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="9"/>
       <c r="I6" s="37" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J6" s="6"/>
       <c r="K6" s="34"/>
@@ -1404,13 +1408,13 @@
     </row>
     <row r="7" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D7" s="29">
         <f>VLOOKUP(C7,Params!$K$2:$N$9,4,FALSE)</f>
@@ -1418,12 +1422,12 @@
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="9"/>
       <c r="I7" s="37" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J7" s="6"/>
       <c r="K7" s="34"/>
@@ -1431,13 +1435,13 @@
     </row>
     <row r="8" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D8" s="29">
         <f>VLOOKUP(C8,Params!$K$2:$N$9,4,FALSE)</f>
@@ -1445,28 +1449,26 @@
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="9"/>
       <c r="I8" s="37" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J8" s="6"/>
       <c r="K8" s="34"/>
-      <c r="L8" s="35">
-        <v>870</v>
-      </c>
+      <c r="L8" s="35"/>
     </row>
     <row r="9" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D9" s="29">
         <f>VLOOKUP(C9,Params!$K$2:$N$9,4,FALSE)</f>
@@ -1474,12 +1476,12 @@
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="9"/>
-      <c r="I9" s="40" t="s">
-        <v>20</v>
+      <c r="I9" s="38" t="s">
+        <v>17</v>
       </c>
       <c r="J9" s="6"/>
       <c r="K9" s="34"/>
@@ -1487,66 +1489,62 @@
     </row>
     <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D10" s="29">
         <f>VLOOKUP(C10,Params!$K$2:$N$9,4,FALSE)</f>
-        <v>60</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>9</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="G10" s="3"/>
       <c r="H10" s="9"/>
-      <c r="I10" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="I10" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="6"/>
       <c r="K10" s="34"/>
-      <c r="L10" s="35"/>
+      <c r="L10" s="35">
+        <v>960</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D11" s="29">
         <f>VLOOKUP(C11,Params!$K$2:$N$9,4,FALSE)</f>
         <v>60</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="G11" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="K11" s="34"/>
       <c r="L11" s="35"/>
@@ -1607,7 +1605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P22"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
@@ -1630,39 +1628,39 @@
   <sheetData>
     <row r="1" spans="2:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="20" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="25" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K2" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="N2" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="O2" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2" s="38"/>
+      <c r="O2" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="P2" s="39"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="26" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="K3" s="22" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="L3" s="23" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="M3" s="24">
         <v>2</v>
@@ -1670,21 +1668,21 @@
       <c r="N3" s="24">
         <v>60</v>
       </c>
-      <c r="O3" s="39" t="str">
+      <c r="O3" s="40" t="str">
         <f>L3 &amp; " fields OR " &amp; M3 &amp; " trans"</f>
         <v>3-5 fields OR 2 trans</v>
       </c>
-      <c r="P3" s="39"/>
+      <c r="P3" s="40"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="26" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K4" s="22" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L4" s="23" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M4" s="24">
         <v>3</v>
@@ -1692,21 +1690,21 @@
       <c r="N4" s="24">
         <v>90</v>
       </c>
-      <c r="O4" s="39" t="str">
+      <c r="O4" s="40" t="str">
         <f t="shared" ref="O4:O9" si="0">L4 &amp; " fields OR " &amp; M4 &amp; " trans"</f>
         <v>6-7 fields OR 3 trans</v>
       </c>
-      <c r="P4" s="39"/>
+      <c r="P4" s="40"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="K5" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L5" s="23" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M5" s="24">
         <v>4</v>
@@ -1714,21 +1712,21 @@
       <c r="N5" s="24">
         <v>120</v>
       </c>
-      <c r="O5" s="39" t="str">
+      <c r="O5" s="40" t="str">
         <f t="shared" si="0"/>
         <v>8-9 fields OR 4 trans</v>
       </c>
-      <c r="P5" s="39"/>
+      <c r="P5" s="40"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="25" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K6" s="22" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="L6" s="23" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="M6" s="24">
         <v>5</v>
@@ -1745,10 +1743,10 @@
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="25"/>
       <c r="K7" s="22" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="L7" s="23" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="M7" s="24">
         <v>6</v>
@@ -1764,13 +1762,13 @@
     </row>
     <row r="8" spans="2:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B8" s="20" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K8" s="22" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="L8" s="23" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="M8" s="24">
         <v>7</v>
@@ -1786,16 +1784,16 @@
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="27" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="K9" s="22" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L9" s="24" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M9" s="24" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="N9" s="24">
         <v>240</v>
@@ -1808,17 +1806,17 @@
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="K10" s="19" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="K14" s="27" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="27" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>